<commit_message>
Se agegó la estructura del  JSON
</commit_message>
<xml_diff>
--- a/Resumen.xlsx
+++ b/Resumen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Sheyla\Clases\BibliotecaVirtual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5507C27-CF20-461C-9707-1A56A3FD7A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA294CE-4162-41E8-B398-F587396FEC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4395" yWindow="3630" windowWidth="22290" windowHeight="12735" xr2:uid="{7D30D357-660E-4334-9EEF-43E8EB787F34}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A2:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>